<commit_message>
[GEN] Block diagram update
</commit_message>
<xml_diff>
--- a/Plasma_RF_Generator_Spec.xlsx
+++ b/Plasma_RF_Generator_Spec.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="1" r:id="rId1"/>
     <sheet name="Check list" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Device Review" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>VAC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -374,6 +374,38 @@
   <si>
     <t>Power Amp 부품 search - 100W 이상
   - recommand : 200W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF AMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRFE6VP61K25H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Part Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vendor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1250W RF Power LDMOS Transistor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,12 +734,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,27 +750,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -757,59 +768,80 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1138,379 +1170,379 @@
     </row>
     <row r="3" spans="2:7" s="4" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8">
+      <c r="C4" s="48"/>
+      <c r="D4" s="6">
         <v>230</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>220</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <v>4</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <v>6.4</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="42"/>
+      <c r="C14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13">
+      <c r="C15" s="12"/>
+      <c r="D15" s="11">
         <v>50</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>50</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <v>120</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="21"/>
-      <c r="C17" s="14" t="s">
+      <c r="B17" s="40"/>
+      <c r="C17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="11">
         <v>200</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="16"/>
+      <c r="F18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="40"/>
+      <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="14" t="s">
+      <c r="E19" s="16"/>
+      <c r="F19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="22" t="s">
+      <c r="C22" s="12"/>
+      <c r="D22" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="14" t="s">
+      <c r="E22" s="16"/>
+      <c r="F22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="15"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="40"/>
+      <c r="C24" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="14" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="15"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="14" t="s">
+      <c r="E25" s="16"/>
+      <c r="F25" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G25" s="15"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="23"/>
-      <c r="C26" s="24" t="s">
+      <c r="B26" s="41"/>
+      <c r="C26" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="24" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="26"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="23" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1521,8 +1553,8 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="32"/>
-      <c r="C28" s="30" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="23" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1536,7 +1568,7 @@
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="23" t="s">
         <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1550,7 +1582,7 @@
       <c r="B30" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="11" t="s">
         <v>74</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1564,17 +1596,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1585,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13:H14"/>
     </sheetView>
   </sheetViews>
@@ -1600,306 +1632,306 @@
   <sheetData>
     <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="43">
+      <c r="B4" s="34">
         <v>1</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="35">
         <v>43252</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="46" t="s">
+      <c r="F4" s="35"/>
+      <c r="G4" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="2:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="37">
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="40" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="2:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="37">
+      <c r="B6" s="28">
         <v>3</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="40" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="37">
+      <c r="B7" s="28">
         <v>4</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="37">
+      <c r="B8" s="28">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="37">
+      <c r="B9" s="28">
         <v>6</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="37">
+      <c r="B10" s="28">
         <v>7</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="37">
+      <c r="B11" s="28">
         <v>8</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="37">
+      <c r="B12" s="28">
         <v>9</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="37">
+      <c r="B13" s="28">
         <v>10</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="37">
+      <c r="B14" s="28">
         <v>11</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="42"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="37">
+      <c r="B15" s="28">
         <v>12</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="37">
+      <c r="B16" s="28">
         <v>13</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="37">
+      <c r="B17" s="28">
         <v>14</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="42"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="37">
+      <c r="B18" s="28">
         <v>15</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="37">
+      <c r="B19" s="28">
         <v>16</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="37">
+      <c r="B20" s="28">
         <v>17</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="42"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="37">
+      <c r="B21" s="28">
         <v>18</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="37">
+      <c r="B22" s="28">
         <v>19</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="33"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="37">
+      <c r="B23" s="28">
         <v>20</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="33"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="37">
+      <c r="B24" s="28">
         <v>21</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="42"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="37">
+      <c r="B25" s="28">
         <v>22</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="42"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1909,12 +1941,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C5:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>